<commit_message>
MockData excel file updated
</commit_message>
<xml_diff>
--- a/MockData.xlsx
+++ b/MockData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\School\Lewis\Software Systems Capstone CPSC-49200-003\Community Charity App\Capstone-Site\my-app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\School\Lewis\Software Systems Capstone CPSC-49200-003\Community Charity App\Capstone-Site\my-app\CapstoneSite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{04414F4E-5D45-40E5-973B-3AFF3D94721D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{012378BF-84C4-4906-BAFD-876DC5A6E45A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33660" yWindow="3285" windowWidth="28800" windowHeight="16605" activeTab="1" xr2:uid="{C9A4CAAC-B9BE-47E9-BACB-D510E8CF2234}"/>
+    <workbookView xWindow="-36090" yWindow="3210" windowWidth="73950" windowHeight="16605" activeTab="1" xr2:uid="{C9A4CAAC-B9BE-47E9-BACB-D510E8CF2234}"/>
   </bookViews>
   <sheets>
     <sheet name="Charity" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="237">
   <si>
     <t>Charity Name</t>
   </si>
@@ -742,6 +742,12 @@
   </si>
   <si>
     <t>Woodland Interiors is an interior design business that offers creative and and stylish solutions to customers in the Romeoville and surrounding areas.</t>
+  </si>
+  <si>
+    <t>INSERT INTO businessuser (`id`,`email`,`businessName`,`password`,`city`,`state`,`zipCode`,`phone`,`description`,`address`,`createdAt`,`updatedAt`)</t>
+  </si>
+  <si>
+    <t>INSERT INTO 'businessuser' (`id`,`email`,`businessName`,`password`,`city`,`state`,`zipCode`,`phone`,`description`,`address`,`createdAt`,`updatedAt`) VALUES (DEFAULT,?,?,?,?,?,?,?,?,?,?,?);</t>
   </si>
 </sst>
 </file>
@@ -1133,8 +1139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09298AC3-31E0-4098-A7A3-ABBE3F2445F3}">
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView topLeftCell="I1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2163,390 +2169,532 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C79CEA9-0714-4CD5-9FEE-666E3E023C94}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:Q46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I13"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="23.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" customWidth="1"/>
+    <col min="7" max="7" width="144.28515625" customWidth="1"/>
+    <col min="8" max="8" width="16" customWidth="1"/>
+    <col min="9" max="9" width="33.140625" customWidth="1"/>
+    <col min="10" max="10" width="3.140625" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B1" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="G1" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    </row>
+    <row r="2" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="5">
+        <v>60601</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="G2" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="P2" t="str">
+        <f>_xlfn.CONCAT("(DEFAULT,'", $I2, "', '", $B2, "', '", $K2, "', '", $D2, "', '", $C2, "', '", $E2,, "', '", $F2, "', '", $G2, "', '", $H2, "', '", $A$26,"', '", $A$26, "'), ")</f>
+        <v xml:space="preserve">(DEFAULT,'atozinc@gmail.com', 'A to Z Inc.', 'Atoz123', 'Chicago', 'IL', '60601', '(312) 555-1234', 'A to Z Inc. is a local business that offers a variety of services including home improvement, landscaping, and cleaning.', '100 Main St', '2023-04-09 01:53:06', '2023-04-09 01:53:06'), </v>
+      </c>
+    </row>
+    <row r="3" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="E3" s="5">
+        <v>60004</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="P3" t="str">
+        <f t="shared" ref="P3:P13" si="0">_xlfn.CONCAT("(DEFAULT,'", $I3, "', '", $B3, "', '", $K3, "', '", $D3, "', '", $C3, "', '", $E3,, "', '", $F3, "', '", $G3, "', '", $H3, "', '", $A$26,"', '", $A$26, "'), ")</f>
+        <v xml:space="preserve">(DEFAULT,'probuildersllc@gmail.com', 'Pro Builders LLC', 'Probuilders456', 'Arlington Heights', 'IL', '60004', '(773) 555-5678', 'Pro Builders LLC is a construction company that specializes in residential and commercial projects in the Arlington Heights area.', '200 State St', '2023-04-09 01:53:06', '2023-04-09 01:53:06'), </v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="E4" s="5">
+        <v>60076</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="P4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">(DEFAULT,'pamperedpawssalon@yahoo.com', 'Pampered Paws Salon', 'Pampered901', 'Skokie', 'IL', '60076', '(847) 555-9012', 'Pampered Paws Salon is a pet grooming business that provides quality services to pet owners in the Skokie community.', '300 Oak Ave', '2023-04-09 01:53:06', '2023-04-09 01:53:06'), </v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="E5" s="5">
+        <v>60540</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="P5" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">(DEFAULT,'vitalitynutrition@yahoo.com', 'Vitality Nutrition', 'Vitality234', 'Naperville', 'IL', '60540', '(312) 555-2345', 'Vitality Nutrition is a health food store that offers a wide selection of organic and natural products to the Naperville community.', '400 Elm St', '2023-04-09 01:53:06', '2023-04-09 01:53:06'), </v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="E6" s="5">
+        <v>60201</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="P6" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">(DEFAULT,'dynamicdesignersinc@gmail.com', 'Dynamic Designers Inc.', 'Dynamic678', 'Evanston', 'IL', '60201', '(847) 555-6789', 'Dynamic Designers Inc. is a web design company that creates innovative and responsive websites for businesses in the Evanston area.', '500 Pine St', '2023-04-09 01:53:06', '2023-04-09 01:53:06'), </v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="E7" s="5">
+        <v>60193</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="P7" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">(DEFAULT,'expresscleaners@gmail.com', 'Express Cleaners', 'Express345', 'Schaumburg', 'IL', '60193', '(224) 555-3456', 'Express Cleaners is a dry cleaning business that provides fast and reliable services to the Schaumburg community.', '600 Maple Rd', '2023-04-09 01:53:06', '2023-04-09 01:53:06'), </v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="E8" s="5">
+        <v>60016</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="P8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">(DEFAULT,'goldcoastjewelry@yahoo.com', 'Gold Coast Jewelry', 'Gold789', 'Des Plaines', 'IL', '60016', '(312) 555-7890', 'Gold Coast Jewelry is a family-owned business that offers a wide selection of fine jewelry to customers in the Des Plaines area.', '700 Oak Ave', '2023-04-09 01:53:06', '2023-04-09 01:53:06'), </v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E9" s="5">
+        <v>60301</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="P9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">(DEFAULT,'urbanbikes@gmail.com', 'Urban Bikes', 'Urban567', 'Oak Park', 'IL', '60301', '(773) 555-5678', 'Urban Bikes is a bike shop that provides quality bikes and accessories to customers in the Oak Park community.', '800 State St', '2023-04-09 01:53:06', '2023-04-09 01:53:06'), </v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="E10" s="5">
+        <v>60004</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="P10" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">(DEFAULT,'thelocalmarket@yahoo.com', 'The Local Market', 'Local901', 'Arlington Heights', 'IL', '60004', '(847) 555-9012', 'The Local Market is a grocery store that offers fresh and locally-sourced products to customers in the Arlington Heights area.', '900 Elm St', '2023-04-09 01:53:06', '2023-04-09 01:53:06'), </v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="E11" s="5">
+        <v>60601</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="P11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">(DEFAULT,'theprintshop@yahoo.com', 'The Print Shop', 'Print234', 'Chicago', 'IL', '60601', '(312) 555-2345', 'The Print Shop is a printing business that offers a variety of services including business cards, flyers, and posters to customers in the Chicago community.', '1000 Main St', '2023-04-09 01:53:06', '2023-04-09 01:53:06'), </v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="5">
-        <v>60601</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="G3" s="5" t="s">
+      <c r="D12" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="E12" s="5">
+        <v>60076</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="P12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">(DEFAULT,'fusionfitness@yahoo.com', 'Fusion Fitness', 'Fusion678', 'Skokie', 'IL', '60076', '(847) 555-6789', 'Fusion Fitness is a gym that offers fitness classes and personal training services to customers in the Skokie area.', '1100 Pine St', '2023-04-09 01:53:06', '2023-04-09 01:53:06'), </v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="5">
-        <v>60004</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="5">
-        <v>60076</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="5">
-        <v>60540</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="F6" s="5" t="s">
+      <c r="D13" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="G6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="5">
+      <c r="E13" s="5">
         <v>60201</v>
       </c>
-      <c r="I6" s="5" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="5">
-        <v>60193</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="B8" s="5" t="s">
+      <c r="F13" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="5">
-        <v>60016</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" s="5">
-        <v>60301</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" s="5">
-        <v>60004</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" s="5">
-        <v>60601</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" s="5">
-        <v>60076</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="C13" s="5" t="s">
+      <c r="G13" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="H13" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="I13" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="K13" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="F13" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H13" s="5">
-        <v>60201</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>234</v>
-      </c>
+      <c r="P13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">(DEFAULT,'woodlandinteriors@gmail.com', 'Woodland Interiors', 'Woodland789', 'Evanston', 'IL', '60201', '(312) 555-7890', 'Woodland Interiors is an interior design business that offers creative and and stylish solutions to customers in the Romeoville and surrounding areas.', '1200 Oak Ave', '2023-04-09 01:53:06', '2023-04-09 01:53:06'), </v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="str">
+        <f>_xlfn.CONCAT("VALUES (DEFAULT,'", $G2, "', '", $F2, "', '", "password", "', '", $I2, "', '", $O35, "', '", $Q35,, "', '", $D2, "', '", $C2, "', '", $A$26,"', '", $A$26, "');")</f>
+        <v>VALUES (DEFAULT,'A to Z Inc. is a local business that offers a variety of services including home improvement, landscaping, and cleaning.', '(312) 555-1234', 'password', 'atozinc@gmail.com', '', '', 'Chicago', 'IL', '2023-04-09 01:53:06', '2023-04-09 01:53:06');</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="str">
+        <f>_xlfn.TEXTJOIN(" ",,P2:P20)</f>
+        <v xml:space="preserve">(DEFAULT,'atozinc@gmail.com', 'A to Z Inc.', 'Atoz123', 'Chicago', 'IL', '60601', '(312) 555-1234', 'A to Z Inc. is a local business that offers a variety of services including home improvement, landscaping, and cleaning.', '100 Main St', '2023-04-09 01:53:06', '2023-04-09 01:53:06'),  (DEFAULT,'probuildersllc@gmail.com', 'Pro Builders LLC', 'Probuilders456', 'Arlington Heights', 'IL', '60004', '(773) 555-5678', 'Pro Builders LLC is a construction company that specializes in residential and commercial projects in the Arlington Heights area.', '200 State St', '2023-04-09 01:53:06', '2023-04-09 01:53:06'),  (DEFAULT,'pamperedpawssalon@yahoo.com', 'Pampered Paws Salon', 'Pampered901', 'Skokie', 'IL', '60076', '(847) 555-9012', 'Pampered Paws Salon is a pet grooming business that provides quality services to pet owners in the Skokie community.', '300 Oak Ave', '2023-04-09 01:53:06', '2023-04-09 01:53:06'),  (DEFAULT,'vitalitynutrition@yahoo.com', 'Vitality Nutrition', 'Vitality234', 'Naperville', 'IL', '60540', '(312) 555-2345', 'Vitality Nutrition is a health food store that offers a wide selection of organic and natural products to the Naperville community.', '400 Elm St', '2023-04-09 01:53:06', '2023-04-09 01:53:06'),  (DEFAULT,'dynamicdesignersinc@gmail.com', 'Dynamic Designers Inc.', 'Dynamic678', 'Evanston', 'IL', '60201', '(847) 555-6789', 'Dynamic Designers Inc. is a web design company that creates innovative and responsive websites for businesses in the Evanston area.', '500 Pine St', '2023-04-09 01:53:06', '2023-04-09 01:53:06'),  (DEFAULT,'expresscleaners@gmail.com', 'Express Cleaners', 'Express345', 'Schaumburg', 'IL', '60193', '(224) 555-3456', 'Express Cleaners is a dry cleaning business that provides fast and reliable services to the Schaumburg community.', '600 Maple Rd', '2023-04-09 01:53:06', '2023-04-09 01:53:06'),  (DEFAULT,'goldcoastjewelry@yahoo.com', 'Gold Coast Jewelry', 'Gold789', 'Des Plaines', 'IL', '60016', '(312) 555-7890', 'Gold Coast Jewelry is a family-owned business that offers a wide selection of fine jewelry to customers in the Des Plaines area.', '700 Oak Ave', '2023-04-09 01:53:06', '2023-04-09 01:53:06'),  (DEFAULT,'urbanbikes@gmail.com', 'Urban Bikes', 'Urban567', 'Oak Park', 'IL', '60301', '(773) 555-5678', 'Urban Bikes is a bike shop that provides quality bikes and accessories to customers in the Oak Park community.', '800 State St', '2023-04-09 01:53:06', '2023-04-09 01:53:06'),  (DEFAULT,'thelocalmarket@yahoo.com', 'The Local Market', 'Local901', 'Arlington Heights', 'IL', '60004', '(847) 555-9012', 'The Local Market is a grocery store that offers fresh and locally-sourced products to customers in the Arlington Heights area.', '900 Elm St', '2023-04-09 01:53:06', '2023-04-09 01:53:06'),  (DEFAULT,'theprintshop@yahoo.com', 'The Print Shop', 'Print234', 'Chicago', 'IL', '60601', '(312) 555-2345', 'The Print Shop is a printing business that offers a variety of services including business cards, flyers, and posters to customers in the Chicago community.', '1000 Main St', '2023-04-09 01:53:06', '2023-04-09 01:53:06'),  (DEFAULT,'fusionfitness@yahoo.com', 'Fusion Fitness', 'Fusion678', 'Skokie', 'IL', '60076', '(847) 555-6789', 'Fusion Fitness is a gym that offers fitness classes and personal training services to customers in the Skokie area.', '1100 Pine St', '2023-04-09 01:53:06', '2023-04-09 01:53:06'),  (DEFAULT,'woodlandinteriors@gmail.com', 'Woodland Interiors', 'Woodland789', 'Evanston', 'IL', '60201', '(312) 555-7890', 'Woodland Interiors is an interior design business that offers creative and and stylish solutions to customers in the Romeoville and surrounding areas.', '1200 Oak Ave', '2023-04-09 01:53:06', '2023-04-09 01:53:06'), </v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="str">
+        <f>_xlfn.CONCAT(A27, " VALUES ", LEFT(A32, LEN(A32)-2),";")</f>
+        <v>INSERT INTO businessuser (`id`,`email`,`businessName`,`password`,`city`,`state`,`zipCode`,`phone`,`description`,`address`,`createdAt`,`updatedAt`) VALUES (DEFAULT,'atozinc@gmail.com', 'A to Z Inc.', 'Atoz123', 'Chicago', 'IL', '60601', '(312) 555-1234', 'A to Z Inc. is a local business that offers a variety of services including home improvement, landscaping, and cleaning.', '100 Main St', '2023-04-09 01:53:06', '2023-04-09 01:53:06'),  (DEFAULT,'probuildersllc@gmail.com', 'Pro Builders LLC', 'Probuilders456', 'Arlington Heights', 'IL', '60004', '(773) 555-5678', 'Pro Builders LLC is a construction company that specializes in residential and commercial projects in the Arlington Heights area.', '200 State St', '2023-04-09 01:53:06', '2023-04-09 01:53:06'),  (DEFAULT,'pamperedpawssalon@yahoo.com', 'Pampered Paws Salon', 'Pampered901', 'Skokie', 'IL', '60076', '(847) 555-9012', 'Pampered Paws Salon is a pet grooming business that provides quality services to pet owners in the Skokie community.', '300 Oak Ave', '2023-04-09 01:53:06', '2023-04-09 01:53:06'),  (DEFAULT,'vitalitynutrition@yahoo.com', 'Vitality Nutrition', 'Vitality234', 'Naperville', 'IL', '60540', '(312) 555-2345', 'Vitality Nutrition is a health food store that offers a wide selection of organic and natural products to the Naperville community.', '400 Elm St', '2023-04-09 01:53:06', '2023-04-09 01:53:06'),  (DEFAULT,'dynamicdesignersinc@gmail.com', 'Dynamic Designers Inc.', 'Dynamic678', 'Evanston', 'IL', '60201', '(847) 555-6789', 'Dynamic Designers Inc. is a web design company that creates innovative and responsive websites for businesses in the Evanston area.', '500 Pine St', '2023-04-09 01:53:06', '2023-04-09 01:53:06'),  (DEFAULT,'expresscleaners@gmail.com', 'Express Cleaners', 'Express345', 'Schaumburg', 'IL', '60193', '(224) 555-3456', 'Express Cleaners is a dry cleaning business that provides fast and reliable services to the Schaumburg community.', '600 Maple Rd', '2023-04-09 01:53:06', '2023-04-09 01:53:06'),  (DEFAULT,'goldcoastjewelry@yahoo.com', 'Gold Coast Jewelry', 'Gold789', 'Des Plaines', 'IL', '60016', '(312) 555-7890', 'Gold Coast Jewelry is a family-owned business that offers a wide selection of fine jewelry to customers in the Des Plaines area.', '700 Oak Ave', '2023-04-09 01:53:06', '2023-04-09 01:53:06'),  (DEFAULT,'urbanbikes@gmail.com', 'Urban Bikes', 'Urban567', 'Oak Park', 'IL', '60301', '(773) 555-5678', 'Urban Bikes is a bike shop that provides quality bikes and accessories to customers in the Oak Park community.', '800 State St', '2023-04-09 01:53:06', '2023-04-09 01:53:06'),  (DEFAULT,'thelocalmarket@yahoo.com', 'The Local Market', 'Local901', 'Arlington Heights', 'IL', '60004', '(847) 555-9012', 'The Local Market is a grocery store that offers fresh and locally-sourced products to customers in the Arlington Heights area.', '900 Elm St', '2023-04-09 01:53:06', '2023-04-09 01:53:06'),  (DEFAULT,'theprintshop@yahoo.com', 'The Print Shop', 'Print234', 'Chicago', 'IL', '60601', '(312) 555-2345', 'The Print Shop is a printing business that offers a variety of services including business cards, flyers, and posters to customers in the Chicago community.', '1000 Main St', '2023-04-09 01:53:06', '2023-04-09 01:53:06'),  (DEFAULT,'fusionfitness@yahoo.com', 'Fusion Fitness', 'Fusion678', 'Skokie', 'IL', '60076', '(847) 555-6789', 'Fusion Fitness is a gym that offers fitness classes and personal training services to customers in the Skokie area.', '1100 Pine St', '2023-04-09 01:53:06', '2023-04-09 01:53:06'),  (DEFAULT,'woodlandinteriors@gmail.com', 'Woodland Interiors', 'Woodland789', 'Evanston', 'IL', '60201', '(312) 555-7890', 'Woodland Interiors is an interior design business that offers creative and and stylish solutions to customers in the Romeoville and surrounding areas.', '1200 Oak Ave', '2023-04-09 01:53:06', '2023-04-09 01:53:06');</v>
+      </c>
+      <c r="O34" s="5"/>
+      <c r="Q34" s="5"/>
+    </row>
+    <row r="35" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="O35" s="5"/>
+      <c r="Q35" s="5"/>
+    </row>
+    <row r="36" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="O36" s="5"/>
+      <c r="Q36" s="5"/>
+    </row>
+    <row r="37" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="O37" s="5"/>
+      <c r="Q37" s="5"/>
+    </row>
+    <row r="38" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="O38" s="5"/>
+      <c r="Q38" s="5"/>
+    </row>
+    <row r="39" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="O39" s="5"/>
+      <c r="Q39" s="5"/>
+    </row>
+    <row r="40" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="O40" s="5"/>
+      <c r="Q40" s="5"/>
+    </row>
+    <row r="41" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="O41" s="5"/>
+      <c r="Q41" s="5"/>
+    </row>
+    <row r="42" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="O42" s="5"/>
+      <c r="Q42" s="5"/>
+    </row>
+    <row r="43" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="O43" s="5"/>
+      <c r="Q43" s="5"/>
+    </row>
+    <row r="44" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="O44" s="5"/>
+      <c r="Q44" s="5"/>
+    </row>
+    <row r="45" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="O45" s="5"/>
+      <c r="Q45" s="5"/>
+    </row>
+    <row r="46" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="O46" s="5"/>
+      <c r="Q46" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
lists improved & indiv pages
</commit_message>
<xml_diff>
--- a/MockData.xlsx
+++ b/MockData.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\School\Lewis\Software Systems Capstone CPSC-49200-003\Community Charity App\Capstone-Site\my-app\CapstoneSite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{012378BF-84C4-4906-BAFD-876DC5A6E45A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3FCA0B2-0E1F-455F-8B11-1EBBD558D373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36090" yWindow="3210" windowWidth="73950" windowHeight="16605" activeTab="1" xr2:uid="{C9A4CAAC-B9BE-47E9-BACB-D510E8CF2234}"/>
+    <workbookView xWindow="-36090" yWindow="3210" windowWidth="27030" windowHeight="16605" activeTab="2" xr2:uid="{C9A4CAAC-B9BE-47E9-BACB-D510E8CF2234}"/>
   </bookViews>
   <sheets>
     <sheet name="Charity" sheetId="1" r:id="rId1"/>
     <sheet name="Business" sheetId="2" r:id="rId2"/>
+    <sheet name="Event" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="265">
   <si>
     <t>Charity Name</t>
   </si>
@@ -748,6 +749,90 @@
   </si>
   <si>
     <t>INSERT INTO 'businessuser' (`id`,`email`,`businessName`,`password`,`city`,`state`,`zipCode`,`phone`,`description`,`address`,`createdAt`,`updatedAt`) VALUES (DEFAULT,?,?,?,?,?,?,?,?,?,?,?);</t>
+  </si>
+  <si>
+    <t>Charity/Business Name</t>
+  </si>
+  <si>
+    <t>Event Name</t>
+  </si>
+  <si>
+    <t>Event Description</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Griggsville Food Drive</t>
+  </si>
+  <si>
+    <t>Come to Griggsville United Methodist Church and donate canned foods and clothing for local communities.</t>
+  </si>
+  <si>
+    <t>Park City Clothing Drive</t>
+  </si>
+  <si>
+    <t>We are organizing a food drive on June 25th. Please come out for music and dancing. Bring any clothes you'd like to donate.</t>
+  </si>
+  <si>
+    <t>Heather's House</t>
+  </si>
+  <si>
+    <t>Heather's House Fundraiser</t>
+  </si>
+  <si>
+    <t>Heather's House is welcoming everyone in the communtiy to come out and join us for a fundraiser. Proceeds will go to local charities.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Montgomery </t>
+  </si>
+  <si>
+    <t>Cemetary Preservation Group Inc.</t>
+  </si>
+  <si>
+    <t>CPG Fundraiser</t>
+  </si>
+  <si>
+    <t>Cemetary Preservation Group Inc. is holding an annual fundraiser on July 3rd.</t>
+  </si>
+  <si>
+    <t>Quincy University Fundraiser</t>
+  </si>
+  <si>
+    <t>Quincy University is hosting a fundraiser for our students in need.</t>
+  </si>
+  <si>
+    <t>LM Food Drive</t>
+  </si>
+  <si>
+    <t>The Local Market is hosting a quarterly food drive for local churches. All donated food will go to local churches that are helping those in need.</t>
+  </si>
+  <si>
+    <t>The Print Shop Clothing Drive</t>
+  </si>
+  <si>
+    <t>The Print Shop welcomes everyone for its' annual clothing drive, please bring any article of clothing you would like to donate.</t>
+  </si>
+  <si>
+    <t>Fusion Fitness's Food Drive</t>
+  </si>
+  <si>
+    <t>Fusion Fitness welcomes everyone for its' annual food drive, please bring any article of food you would like to donate.</t>
+  </si>
+  <si>
+    <t>Woodland Interiors Fundraiser</t>
+  </si>
+  <si>
+    <t>Woodland Interiors is hosting its quarterly fundraiser for local schools. All donated proceeds will go to oodlandlpings in need.</t>
+  </si>
+  <si>
+    <t>Vitality Nutrition Food Drive</t>
+  </si>
+  <si>
+    <t>Vitality Nutrition welcomes everyone for its' annual food drive, please bring any article of food you would like to donate.</t>
   </si>
 </sst>
 </file>
@@ -812,7 +897,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -821,6 +906,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -2171,7 +2257,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C79CEA9-0714-4CD5-9FEE-666E3E023C94}">
   <dimension ref="A1:Q46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
@@ -2699,4 +2785,289 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{078DD25C-182C-47E1-B2C2-C3B073F69B47}">
+  <dimension ref="A1:H1048576"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.7109375" customWidth="1"/>
+    <col min="2" max="2" width="29.85546875" customWidth="1"/>
+    <col min="3" max="3" width="115.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>242</v>
+      </c>
+      <c r="C2" t="s">
+        <v>243</v>
+      </c>
+      <c r="D2" s="6">
+        <v>45097</v>
+      </c>
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2">
+        <v>62340</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
+        <v>244</v>
+      </c>
+      <c r="C3" t="s">
+        <v>245</v>
+      </c>
+      <c r="D3" s="6">
+        <v>45102</v>
+      </c>
+      <c r="F3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3">
+        <v>61115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>246</v>
+      </c>
+      <c r="B4" t="s">
+        <v>247</v>
+      </c>
+      <c r="C4" t="s">
+        <v>248</v>
+      </c>
+      <c r="D4" s="6">
+        <v>45107</v>
+      </c>
+      <c r="F4" t="s">
+        <v>249</v>
+      </c>
+      <c r="G4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4">
+        <v>36110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>250</v>
+      </c>
+      <c r="B5" t="s">
+        <v>251</v>
+      </c>
+      <c r="C5" t="s">
+        <v>252</v>
+      </c>
+      <c r="D5" s="6">
+        <v>45110</v>
+      </c>
+      <c r="F5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H5">
+        <v>36701</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
+        <v>253</v>
+      </c>
+      <c r="C6" t="s">
+        <v>254</v>
+      </c>
+      <c r="D6" s="6">
+        <v>45115</v>
+      </c>
+      <c r="F6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6">
+        <v>62301</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="B7" t="s">
+        <v>255</v>
+      </c>
+      <c r="C7" t="s">
+        <v>256</v>
+      </c>
+      <c r="D7" s="6">
+        <v>45119</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="5">
+        <v>60004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="B8" t="s">
+        <v>257</v>
+      </c>
+      <c r="C8" t="s">
+        <v>258</v>
+      </c>
+      <c r="D8" s="6">
+        <v>45122</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="5">
+        <v>60601</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="B9" t="s">
+        <v>259</v>
+      </c>
+      <c r="C9" t="s">
+        <v>260</v>
+      </c>
+      <c r="D9" s="6">
+        <v>45127</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="5">
+        <v>60076</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B10" t="s">
+        <v>261</v>
+      </c>
+      <c r="C10" t="s">
+        <v>262</v>
+      </c>
+      <c r="D10" s="6">
+        <v>45129</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="5">
+        <v>60201</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B11" t="s">
+        <v>263</v>
+      </c>
+      <c r="C11" t="s">
+        <v>264</v>
+      </c>
+      <c r="D11" s="6">
+        <v>45148</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="5">
+        <v>60540</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D12" s="6"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D13" s="6"/>
+    </row>
+    <row r="1048576" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D1048576" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>